<commit_message>
bottom of syllabus will only be readings
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -412,7 +412,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lab 0: Test submitting a lab</t>
+          <t>Lab 0: Getting started w/ Jupyter notebook / test submitting a lab</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Hwk 1: Collecting personal network survey data</t>
         </is>
       </c>
     </row>
@@ -424,12 +429,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Lab 1: Getting started w/ Jupyter notebooks; working with complete network data</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Hwk 1: Collecting personal network survey data</t>
+          <t>Lab 1: Analyzing personal network data; review of bootstrap</t>
         </is>
       </c>
     </row>
@@ -463,12 +463,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Lab 2: Review of bootstrap, analyzing personal network data</t>
+          <t>Lab 2: Getting started with complete network data</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Hwk 2: Analyzing personal network surveys</t>
+          <t>Hwk 2: Analyzing personal network data</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hwk 3: TODO - Jupyter-based, hypothesis test</t>
+          <t>Hwk 3: Complete network data</t>
         </is>
       </c>
     </row>
@@ -531,12 +531,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>TODO - Lab 4, maybe small worlds?</t>
+          <t>Lab 4 - Exploring mathematical models</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Hwk 4: TODO - written hwk, including graph theory + mathematical models?</t>
+          <t>Hwk 4: Problem set I</t>
         </is>
       </c>
     </row>
@@ -555,12 +555,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>TODO - two-mode network lab/hwk?</t>
+          <t>Lab 5 - Two-mode networks; the friendship paradox</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Hwk 5: ? Small worlds</t>
+          <t>Hwk 5: Advanced complete network data</t>
         </is>
       </c>
     </row>
@@ -587,42 +587,47 @@
           <t>netlogo ba model</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Midterm review / question session</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Hwk 6: Problem set II</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="D14" t="inlineStr">
         <is>
-          <t>Community detection</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Community detection</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>TODO - paper review?</t>
+          <t>Midterm review</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>Empirical studies of network structure</t>
+          <t>Midterm</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="D16" t="inlineStr">
         <is>
-          <t>Midterm review</t>
+          <t>Community detection</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Community detection</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
         <is>
-          <t>Midterm</t>
+          <t>Empirical studies of network structure</t>
         </is>
       </c>
     </row>
@@ -642,11 +647,6 @@
           <t>SIR thresh demo</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Lab X: Centrality and the SIR model</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
@@ -659,6 +659,16 @@
           <t>SIR demo; Network SIR demo</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Lab 6: Simple contagion</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Hwk 7: Centrality and the SIR model</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
@@ -666,16 +676,6 @@
           <t>Sexual networks, concurrency, and HIV</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>TODO - paper review?</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Hwk X: TODO adapt betweenness - written hwk on centrality?</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
@@ -683,6 +683,16 @@
           <t>Empirical studies of simple contagion</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Lab 7: Mini-project prep</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Mini-project</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -695,11 +705,6 @@
           <t>Social influence, herding, and cascades</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>TODO - lab on contagion / maybe cooperation?</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
@@ -707,6 +712,11 @@
           <t>Threshold models and complex contagion</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Mini-project support</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="D24" t="inlineStr">
@@ -714,11 +724,6 @@
           <t>Complex contagion on networks</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>TODO Hwk - complex contagion</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="D25" t="inlineStr">
@@ -726,6 +731,11 @@
           <t>Complex contagion on networks, cont.</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Hwk 8: Problem set III</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
@@ -756,7 +766,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>TODO - paper review?</t>
+          <t>Problem set + mini-project support</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
just readings at bottom of syllabus
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -485,6 +485,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>[Models of network structure](#sec:models)</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>Intro to mathematical network models; the Erdos-Renyi model and its predictions</t>
@@ -519,28 +524,28 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Network centrality / the Friendship Paradox</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Lab 4 - Exploring mathematical models</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Hwk 4: Problem set I</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>[Small worlds](#sec:smallworlds)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Network centrality / the Friendship Paradox</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Lab 4 - Exploring mathematical models</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Hwk 4: Problem set I</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
       <c r="D10" t="inlineStr">
         <is>
           <t>Small worlds</t>
@@ -671,6 +676,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>[Concurrency](#sec:concurrency)</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>Sexual networks, concurrency, and HIV</t>
@@ -697,7 +707,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>[Dynamics: Complex contagion and social influence](#sec:complexcontagion)</t>
+          <t>[Social influence](#sec:socialinfluence)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -719,6 +729,11 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>[Dynamics: Complex contagion and social influence](#sec:complexcontagion)</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>Complex contagion on networks</t>

</xml_diff>

<commit_message>
added links to assignments in syllabus
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -412,12 +412,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lab 0: Getting started w/ Jupyter notebook / test submitting a lab</t>
+          <t>[Lab 0: Getting started w/ Jupyter notebook / test submitting a lab](https://github.com/dfeehan/demog180-fa2024/blob/main/labs/lab0/lab0-rev.ipynb)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Hwk 1: Collecting personal network survey data</t>
+          <t>[Hwk 1: Collecting personal network survey data](https://docs.google.com/document/d/1Og5dk6vW0IH6k_M5otwkGs_s2hhzuF4AaF3Dpexijrs/edit)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added link to homework 2
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Triadic closure, strength of weak ties</t>
+          <t>Triadic closure</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -450,11 +450,16 @@
  [Triadic closure in an email network](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2024%2Flecture%2F20240905_triadic_closure%2Femail-eu-core.ipynb)</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[Hwk 2: Analyzing personal network data](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Fhwk%2Fhwk02%2Fhwk02.ipynb)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>Social capital and structural holes</t>
+          <t>Strength of Weak Ties, Social Capital, Structural Holes</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -477,11 +482,6 @@
       <c r="E6" t="inlineStr">
         <is>
           <t>TODO</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Hwk 2: Analyzing personal network data</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated syllabus with link to homework 3
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -484,6 +484,11 @@
           <t>TODO</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[Hwk 3: Complete network data](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Fhwk%2Fhwk03%2Fhwk03.ipynb)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="D7" t="inlineStr">

</xml_diff>

<commit_message>
link to lecture demo for today
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -510,12 +510,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Structural balance demo</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Hwk 3: Complete network data</t>
+          <t>[Structural balance demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flecture%2F20240919_structural_balance%2Fstructural_balance_in_the_small_slashdot_network.ipynb)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added link to hwk4 = psI
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -532,36 +532,26 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>[Small worlds](#sec:smallworlds)</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Small worlds</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Hwk 4: Problem set I</t>
+          <t>[Hwk 4: Problem set I](https://drive.google.com/file/d/1TUta8-8redraG0L044teOdA3SxX2eBtj/view?usp=sharing)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>[Small worlds](#sec:smallworlds)</t>
-        </is>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>Search in small worlds</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>TODO</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">

</xml_diff>

<commit_message>
added link to lab5 on syllabus
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -400,6 +400,11 @@
           <t>[Intro + Personal Networks](#sec:intro)</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Intro / what social networks are / basic graph theory / class info</t>
@@ -517,7 +522,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ER random networks demo</t>
+          <t>[ER random networks demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flecture%2F20240923_er_random_networks%2Fer_random_networks.ipynb)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -527,41 +532,31 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>[Small worlds](#sec:smallworlds)</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Small worlds</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Hwk 4: Problem set I</t>
+          <t>[Hwk 4: Problem set I](https://drive.google.com/file/d/1TUta8-8redraG0L044teOdA3SxX2eBtj/view?usp=sharing)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>[Small worlds](#sec:smallworlds)</t>
-        </is>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>Search in small worlds</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Lab 5 - Two-mode networks</t>
+          <t>[Lab 5 - Two-mode networks](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab05%2Flab05_two_mode_networks.ipynb)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update syllabus links for lecture demos
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -646,7 +646,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>SIR thresh demo</t>
+          <t>[SIR demo](https://shiny.demog.berkeley.edu/dennis/model-SIR/)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SIR demo; Network SIR demo</t>
+          <t>[Network SIR demo](https://shiny.demog.berkeley.edu/dennis/shiny-SimNetwork/); [Threshold infectiousness demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flecture%2F20241029_sir_threshold_infectiousness%2Fsir_threshold_infectiousness.ipynb)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>? Concurrency demo</t>
+          <t>[Concurrency demo](https://shiny.demog.berkeley.edu/dennis/concurrency/)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">

</xml_diff>

<commit_message>
added lab8 to syllabus
</commit_message>
<xml_diff>
--- a/syllabus/demog180 - 2024.xlsx
+++ b/syllabus/demog180 - 2024.xlsx
@@ -702,7 +702,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Lab 8: Mini-project prep</t>
+          <t>[Lab 8: Mini-project prep](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab08%2Flab08_project_prep.ipynb)</t>
         </is>
       </c>
     </row>
@@ -750,14 +750,14 @@
     <row r="25">
       <c r="D25" t="inlineStr">
         <is>
-          <t>Complex contagion on networks, cont.</t>
+          <t>TBD - likely guest lecture</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Complex contagion on networks, cont.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">

</xml_diff>